<commit_message>
Fix the invalid field names
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -37,11 +37,6 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t/>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="1">
-      <text>
         <t>(Required) HuBMAP ID (e.g., HBM765.TRHD.452) of the sample (i.e., block, section
 or suspension) used to perform this assay. For example, for a RNAseq assay, the
 parent would be the suspension, whereas this would be the HuBMAP ID of a section
@@ -49,7 +44,7 @@
 then this should be a comma separated list.</t>
       </text>
     </comment>
-    <comment ref="C1" authorId="1">
+    <comment ref="B1" authorId="1">
       <text>
         <t>An internal field labs can use it to add whatever ID(s) they want or need for
 dataset validation and tracking. This could be a single ID (e.g.,
@@ -59,32 +54,32 @@
 provider are also used by another.</t>
       </text>
     </comment>
+    <comment ref="C1" authorId="1">
+      <text>
+        <t>DOI for the protocols.io page that describes the assay or sample procurment and
+preparation. For example for an imaging assay, the protocol might include
+staining of a section through the creation of an OME-TIFF file. In this case the
+protocol would include any image processing steps required to create the
+OME-TIFF file.</t>
+      </text>
+    </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might include staining of a section through the creation of an OME-TIFF file. In
-this case the protocol would include any image processing steps required to
-create the OME-TIFF file.</t>
+        <t>(Required) The specific type of dataset being produced.</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
-      <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="1">
       <text>
         <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
 detection/measurement by the assay. The CODEX analyte is protein.</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="1">
+    <comment ref="G1" authorId="1">
       <text>
         <t>(Required) An acquisition instrument is the device that contains the signal
 detection hardware and signal processing software. Assays generate signals such
@@ -92,7 +87,7 @@
 mass.</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1">
+    <comment ref="H1" authorId="1">
       <text>
         <t>(Required) Manufacturers of an acquisition instrument may offer various versions
 (models) of that instrument with different features or sensitivities.
@@ -100,36 +95,36 @@
 interpretation of the data.</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="1">
+    <comment ref="I1" authorId="1">
       <text>
         <t>(Required) How long was the source material (parent) stored, prior to this
 sample being processed.</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="1">
+    <comment ref="J1" authorId="1">
       <text>
         <t>(Required) The time duration unit of measurement</t>
       </text>
     </comment>
-    <comment ref="L1" authorId="1">
+    <comment ref="K1" authorId="1">
       <text>
         <t>The amount of time since the acqusition instrument was last serviced by the
 vendor. This provides a metric for assessing drift in data capture.</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="1">
+    <comment ref="L1" authorId="1">
       <text>
         <t>The time unit of measurement</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="1">
+    <comment ref="M1" authorId="1">
       <text>
         <t>(Required) The path to the file with the ORCID IDs for all contributors of this
 dataset (e.g., "extras/contributors.tsv" or "./contributors.tsv"). This is an
 internal metadata field that is just used for ingest.</t>
       </text>
     </comment>
-    <comment ref="O1" authorId="1">
+    <comment ref="N1" authorId="1">
       <text>
         <t>(Required) The top level directory containing the raw and/or processed data. For
 a single dataset upload this might be "." where as for a data upload containing
@@ -141,21 +136,21 @@
 used for ingest.</t>
       </text>
     </comment>
-    <comment ref="P1" authorId="1">
+    <comment ref="O1" authorId="1">
       <text>
         <t>Depending on if the acquisition instrument was a microscope, slide scanner, etc.
 will indicate whether or not any level of preprocessing was required to assemble
 the image (e.g., fusing image tiles) .</t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1">
+    <comment ref="P1" authorId="1">
       <text>
         <t>(Required) The name of the chemical stains (dyes) applied to histology samples
 to highlight important features of the tissue as well as to enhance the tissue
 contrast.</t>
       </text>
     </comment>
-    <comment ref="R1" authorId="1">
+    <comment ref="Q1" authorId="1">
       <text>
         <t>There are typically three types of stains: progressive, modified progressive,
 and regressive. Progressive staining occurs when the hematoxylin is added to the
@@ -163,31 +158,31 @@
 regressive and modified progressive staining, a differentiator is used.</t>
       </text>
     </comment>
-    <comment ref="S1" authorId="1">
+    <comment ref="R1" authorId="1">
       <text>
         <t>(Required) Are the slides stained using a linear batch method or individually?</t>
       </text>
     </comment>
-    <comment ref="T1" authorId="1">
+    <comment ref="S1" authorId="1">
       <text>
         <t>(Required) Is the slide staining automated with an instrument?</t>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="T1" authorId="1">
       <text>
         <t>The manufacturer of the instrument used to prepare (staining/processing) the
 sample for the assay. If an automatic slide staining method was indicated this
 field should list the manufacturer of the instrument.</t>
       </text>
     </comment>
-    <comment ref="V1" authorId="1">
+    <comment ref="U1" authorId="1">
       <text>
         <t>Manufacturers of a staining system instrument may offer various versions
 (models) of that instrument with different features. Differences in features or
 sensitivities may be relevant to processing or interpretation of the data.</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="1">
+    <comment ref="V1" authorId="1">
       <text>
         <t>A unique ID denoting the slide used. This allows users the ability to determine
 which tissue sections were processed together on the same slide. It is
@@ -195,36 +190,36 @@
 values overlapping across centers.</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="1">
+    <comment ref="W1" authorId="1">
       <text>
         <t>This is how the tiles are configured for stitching.</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1">
+    <comment ref="X1" authorId="1">
       <text>
         <t>This is the direction of imaging, which is required for stitching.</t>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1">
+    <comment ref="Y1" authorId="1">
       <text>
         <t>This is how many columns used in stitching. This is sometimes referred to as the
 grid size x.</t>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1">
+    <comment ref="Z1" authorId="1">
       <text>
         <t>This is the total number of raw (tiled) images captured, that are to be stitched
 together.</t>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1">
+    <comment ref="AA1" authorId="1">
       <text>
         <t>The amount of overlap between tiled images. This is the set point, where as
 during image acquisition there will be slight variations due to stage
 registration.</t>
       </text>
     </comment>
-    <comment ref="AC1" authorId="1">
+    <comment ref="AB1" authorId="1">
       <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
@@ -236,17 +231,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="282">
-  <si>
-    <t>header_info</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="286">
   <si>
     <t>parent_sample_id</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>lab_id</t>
   </si>
   <si>
@@ -961,6 +950,12 @@
     <t>preparation_instrument_model</t>
   </si>
   <si>
+    <t>Chromium X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_999998</t>
+  </si>
+  <si>
     <t>Sublimator</t>
   </si>
   <si>
@@ -979,6 +974,18 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>Chromium Controller</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019326</t>
+  </si>
+  <si>
+    <t>Chromium iX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_999999</t>
+  </si>
+  <si>
     <t>M5 Sprayer</t>
   </si>
   <si>
@@ -1075,7 +1082,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-09-23T12:05:42-07:00</t>
+    <t>2023-10-03T09:54:49-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1134,12 +1141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1178,41 +1184,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="11.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="2" max="2" style="3" width="16.6875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="6.33984375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="23.45703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="12.28515625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="12.66796875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="10.8984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="28.46484375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="27.87109375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="28.5625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="27.40234375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="47.64453125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="14" width="46.48828125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" style="15" width="16.90625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="9.81640625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="30.79296875" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="11.14453125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="15.02734375" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="21.73828125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="21.0" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="29.08203125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="28.48828125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" style="24" width="7.8125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" style="25" width="16.65625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" style="26" width="13.859375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" style="27" width="19.734375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" style="28" width="17.2421875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" style="29" width="30.83203125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" style="30" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="16.6875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="6.33984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="23.45703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="12.28515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="12.66796875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="10.8984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="28.46484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="27.87109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="28.5625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="27.40234375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="47.64453125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="46.48828125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="14" width="16.90625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" style="15" width="9.81640625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="30.79296875" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="11.14453125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="15.02734375" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="21.73828125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="21.0" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="29.08203125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="28.48828125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="7.8125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" style="24" width="16.65625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" style="25" width="13.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" style="26" width="19.734375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" style="27" width="17.2421875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" style="28" width="30.83203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" style="29" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1223,165 +1228,159 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="1">
-        <v>4</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="L1" t="s" s="1">
+        <v>207</v>
+      </c>
+      <c r="M1" t="s" s="1">
         <v>208</v>
       </c>
-      <c r="M1" t="s" s="1">
+      <c r="N1" t="s" s="1">
         <v>209</v>
       </c>
-      <c r="N1" t="s" s="1">
+      <c r="O1" t="s" s="1">
         <v>210</v>
       </c>
-      <c r="O1" t="s" s="1">
+      <c r="P1" t="s" s="1">
         <v>211</v>
       </c>
-      <c r="P1" t="s" s="1">
-        <v>212</v>
-      </c>
       <c r="Q1" t="s" s="1">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="S1" t="s" s="1">
+        <v>230</v>
+      </c>
+      <c r="T1" t="s" s="1">
         <v>231</v>
       </c>
-      <c r="T1" t="s" s="1">
-        <v>232</v>
-      </c>
       <c r="U1" t="s" s="1">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>272</v>
-      </c>
-      <c r="AC1" t="s" s="1">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>274</v>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
-    <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$10</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$14</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_model'!$A$1:$A$32</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
-    <dataValidation type="list" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
-    <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'stain_name'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'stain_technique'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_batch_staining_done'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_staining_automated'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="list" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="V2:V1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$9</formula1>
+    <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'preparation_instrument_model'!$A$1:$A$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'tile_configuration'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'tile_configuration'!$A$1:$A$5</formula1>
+      <formula1>'scan_direction'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'scan_direction'!$A$1:$A$5</formula1>
+    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 1" showErrorMessage="true">
+      <formula1>1</formula1>
+      <formula2/>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 1" showErrorMessage="true">
       <formula1>1</formula1>
       <formula2/>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 1" showErrorMessage="true">
-      <formula1>1</formula1>
-      <formula2/>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
@@ -1402,34 +1401,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1447,34 +1446,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1492,12 +1491,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1515,12 +1514,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1538,42 +1537,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +1582,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1591,74 +1590,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>251</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1676,42 +1699,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1729,42 +1752,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1788,30 +1811,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1829,290 +1852,290 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2130,82 +2153,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2223,12 +2246,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2246,114 +2269,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2371,258 +2394,258 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2640,42 +2663,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2693,26 +2716,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2730,12 +2753,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename restricted_files to non_global_files
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -1135,7 +1135,7 @@
     <t>intended_tile_overlap_percentage</t>
   </si>
   <si>
-    <t>restricted_files</t>
+    <t>non_global_files</t>
   </si>
   <si>
     <t>metadata_schema_id</t>
@@ -1156,7 +1156,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-08T12:35:14-08:00</t>
+    <t>2024-01-09T12:04:36-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1292,7 +1292,7 @@
     <col min="25" max="25" style="26" width="19.734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" style="27" width="17.2421875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" style="28" width="30.83203125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" style="29" width="14.12109375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" style="29" width="15.46484375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" style="30" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added 'ST5020 Multistainer' as an option for 'preparation instrument model'
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="329">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -637,6 +637,12 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
@@ -766,6 +772,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -1105,6 +1117,12 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>ST5020 Multistainer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025021</t>
+  </si>
+  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -1210,7 +1228,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-29T14:12:04-08:00</t>
+    <t>2024-02-21T09:26:06-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1373,70 +1391,70 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
@@ -1444,7 +1462,7 @@
         <v>46</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -1459,10 +1477,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$46</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1497,7 +1515,7 @@
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'tile_configuration'!$A$1:$A$5</formula1>
@@ -1534,34 +1552,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1579,34 +1597,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1686,26 +1704,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6">
@@ -1718,10 +1736,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1749,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1739,114 +1757,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>290</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -1864,42 +1890,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -1917,42 +1943,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -1976,16 +2002,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
@@ -1993,13 +2019,13 @@
         <v>46</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2410,7 +2436,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2568,6 +2594,14 @@
         <v>134</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2575,7 +2609,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2583,362 +2617,370 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2956,42 +2998,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3009,26 +3051,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "PhenoImager Fusion" in the acquisition instrument model
Closes #1
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="331">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -712,6 +712,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
     <t>DM6 B</t>
   </si>
   <si>
@@ -1228,7 +1234,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-21T09:26:06-08:00</t>
+    <t>2024-02-27T07:09:34-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1394,67 +1400,67 @@
         <v>137</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2">
@@ -1462,7 +1468,7 @@
         <v>46</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1486,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$46</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$47</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1552,34 +1558,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -1597,34 +1603,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -1704,26 +1710,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6">
@@ -1736,10 +1742,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -1765,114 +1771,114 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1890,42 +1896,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1943,42 +1949,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2002,16 +2008,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2">
@@ -2019,13 +2025,13 @@
         <v>46</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2609,7 +2615,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2981,6 +2987,14 @@
       </c>
       <c r="B46" t="s" s="0">
         <v>229</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2998,42 +3012,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3051,26 +3065,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Aperio AT2" in the acquisition instrument model
Closes #4
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="333">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -868,6 +868,12 @@
     <t>https://identifiers.org/RRID:SCR_023617</t>
   </si>
   <si>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
+  </si>
+  <si>
     <t>MIBIscope</t>
   </si>
   <si>
@@ -1234,7 +1240,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-27T07:09:34-08:00</t>
+    <t>2024-02-29T07:09:52-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1400,67 +1406,67 @@
         <v>137</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
@@ -1468,7 +1474,7 @@
         <v>46</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1492,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$47</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1558,34 +1564,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1603,34 +1609,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1710,26 +1716,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6">
@@ -1742,10 +1748,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -1771,114 +1777,114 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1896,42 +1902,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -1949,42 +1955,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2008,16 +2014,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
@@ -2025,13 +2031,13 @@
         <v>46</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2615,7 +2621,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2995,6 +3001,14 @@
       </c>
       <c r="B47" t="s" s="0">
         <v>231</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3012,42 +3026,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3065,26 +3079,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "EVOS M7000" in the acquisition instrument model
Closes #7
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="339">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -358,6 +358,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -463,6 +469,12 @@
     <t>analyte_class</t>
   </si>
   <si>
+    <t>DNA + RNA</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -682,30 +694,144 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
-  </si>
-  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -724,36 +850,12 @@
     <t>https://identifiers.org/RRID:SCR_024857</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
     <t>Phenocycler-Fusion 2.0</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
-  </si>
-  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -766,12 +868,6 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
@@ -814,12 +910,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -832,42 +922,12 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
-  </si>
-  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -880,18 +940,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -904,36 +952,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1240,7 +1258,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-29T07:09:52-08:00</t>
+    <t>2024-03-05T18:33:51-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1394,96 +1412,96 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
@@ -1492,7 +1510,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1564,34 +1582,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1609,34 +1627,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -1654,12 +1672,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1677,12 +1695,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1700,58 +1718,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -1769,122 +1787,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>145</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>213</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -1902,42 +1920,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -1955,42 +1973,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2014,30 +2032,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2065,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2317,6 +2335,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2324,7 +2350,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2332,90 +2358,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2433,12 +2467,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2456,162 +2490,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2621,7 +2655,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2629,386 +2663,394 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3026,42 +3068,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3079,26 +3121,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3116,12 +3158,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'H-DAB' as a new stain name
Closes #10
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="341">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1042,6 +1042,12 @@
     <t>http://purl.bioontology.org/ontology/LNC/LP6443-8</t>
   </si>
   <si>
+    <t>H-DAB</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000329</t>
+  </si>
+  <si>
     <t>H&amp;E</t>
   </si>
   <si>
@@ -1258,7 +1264,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-05T18:33:51-08:00</t>
+    <t>2024-03-12T09:43:34-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1448,43 +1454,43 @@
         <v>257</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2">
@@ -1492,7 +1498,7 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1536,7 @@
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'stain_name'!$A$1:$A$4</formula1>
+      <formula1>'stain_name'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'stain_technique'!$A$1:$A$4</formula1>
@@ -1574,7 +1580,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1610,6 +1616,14 @@
       </c>
       <c r="B4" t="s" s="0">
         <v>265</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1627,34 +1641,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -1734,26 +1748,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6">
@@ -1766,10 +1780,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1795,26 +1809,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5">
@@ -1835,74 +1849,74 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1920,42 +1934,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -1973,42 +1987,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -2032,16 +2046,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
@@ -2049,13 +2063,13 @@
         <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Roche Diagnostics' and 'Discovery Ultra' to the acquisition instrument
Closes #11
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="345">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -583,6 +583,12 @@
     <t>https://identifiers.org/RRID:SCR_008452</t>
   </si>
   <si>
+    <t>Roche Diagnostics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025096</t>
+  </si>
+  <si>
     <t>Zeiss Microscopy</t>
   </si>
   <si>
@@ -742,6 +748,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
   </si>
   <si>
+    <t>Discovery Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025097</t>
+  </si>
+  <si>
     <t>Q Exactive UHMR</t>
   </si>
   <si>
@@ -1264,7 +1276,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-12T09:43:34-07:00</t>
+    <t>2024-03-14T10:56:04-04:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1427,70 +1439,70 @@
         <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2">
@@ -1498,7 +1510,7 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -1513,10 +1525,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1588,42 +1600,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1641,34 +1653,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1740,50 +1752,50 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -1801,122 +1813,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -1934,42 +1946,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -1987,42 +1999,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2046,16 +2058,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
@@ -2063,13 +2075,13 @@
         <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -2496,7 +2508,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2662,6 +2674,14 @@
         <v>140</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2669,7 +2689,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2677,394 +2697,402 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3082,42 +3110,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3135,26 +3163,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'EVOS M7000' in the acquisition instrument model.
Closes #22
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="347">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -700,30 +700,144 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
-  </si>
-  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -742,36 +856,12 @@
     <t>https://identifiers.org/RRID:SCR_024857</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
     <t>Phenocycler-Fusion 2.0</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
-  </si>
-  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -784,12 +874,6 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
@@ -832,12 +916,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -850,42 +928,12 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
-  </si>
-  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -898,18 +946,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -922,36 +958,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1123,12 +1129,6 @@
     <t>https://identifiers.org/RRID:SCR_023729</t>
   </si>
   <si>
-    <t>EVOS M7000</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_025070</t>
-  </si>
-  <si>
     <t>Chromium Controller</t>
   </si>
   <si>
@@ -1282,7 +1282,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-19T12:41:40-07:00</t>
+    <t>2024-03-25T11:32:49-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1448,43 +1448,43 @@
         <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="V1" t="s" s="1">
         <v>315</v>
@@ -1534,7 +1534,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1606,42 +1606,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1659,34 +1659,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
@@ -1782,26 +1782,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8">
@@ -1814,10 +1814,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -1835,34 +1835,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>151</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>291</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>292</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5">
@@ -1875,18 +1875,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>219</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8">
@@ -2000,10 +2000,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
@@ -2061,10 +2061,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5">
@@ -2727,7 +2727,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3115,6 +3115,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>239</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3132,42 +3140,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3185,26 +3193,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'BZ-X810' in the acquisition instrument model
Closes #24
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="351">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -832,6 +832,12 @@
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
+    <t>BZ-X810</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025160</t>
+  </si>
+  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
@@ -1183,6 +1189,12 @@
     <t>https://identifiers.org/RRID:SCR_024536</t>
   </si>
   <si>
+    <t>Chromium Connect</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025146</t>
+  </si>
+  <si>
     <t>M5 Sprayer</t>
   </si>
   <si>
@@ -1282,7 +1294,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-25T11:32:49-07:00</t>
+    <t>2024-03-28T12:38:24-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1448,67 +1460,67 @@
         <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2">
@@ -1516,7 +1528,7 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1546,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1569,7 +1581,7 @@
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$17</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'tile_configuration'!$A$1:$A$5</formula1>
@@ -1606,42 +1618,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1659,34 +1671,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1766,10 +1778,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
@@ -1782,26 +1794,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8">
@@ -1814,10 +1826,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1827,7 +1839,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1843,18 +1855,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4">
@@ -1867,10 +1879,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6">
@@ -1883,90 +1895,98 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -1984,42 +2004,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2037,42 +2057,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2096,16 +2116,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
@@ -2113,13 +2133,13 @@
         <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +2747,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3123,6 +3143,14 @@
       </c>
       <c r="B49" t="s" s="0">
         <v>241</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3140,42 +3168,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3193,26 +3221,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Aperio CS2' in acquisition instrument model
Closes #26
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="353">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -868,6 +868,12 @@
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
+    <t>Aperio CS2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025111</t>
+  </si>
+  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -1294,7 +1300,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-28T12:38:24-07:00</t>
+    <t>2024-03-29T08:05:13-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1460,67 +1466,67 @@
         <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2">
@@ -1528,7 +1534,7 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1552,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$50</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$51</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1618,42 +1624,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1671,34 +1677,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -1778,10 +1784,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
@@ -1794,26 +1800,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8">
@@ -1826,10 +1832,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -1855,18 +1861,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4">
@@ -1879,10 +1885,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6">
@@ -1895,98 +1901,98 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2004,42 +2010,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2057,42 +2063,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2116,16 +2122,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
@@ -2133,13 +2139,13 @@
         <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -2747,7 +2753,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3151,6 +3157,14 @@
       </c>
       <c r="B50" t="s" s="0">
         <v>243</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3168,42 +3182,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3221,26 +3235,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added AB-PAS in stain name
Closes #40
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="357">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1066,6 +1066,12 @@
     <t>http://purl.bioontology.org/ontology/LNC/LP6443-8</t>
   </si>
   <si>
+    <t>AB-PAS</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/LNC/LP6121-0</t>
+  </si>
+  <si>
     <t>H-DAB</t>
   </si>
   <si>
@@ -1306,7 +1312,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-01T14:48:32-07:00</t>
+    <t>2024-05-09T13:10:41-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1496,43 +1502,43 @@
         <v>265</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2">
@@ -1540,7 +1546,7 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1578,7 +1584,7 @@
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'stain_name'!$A$1:$A$5</formula1>
+      <formula1>'stain_name'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'stain_technique'!$A$1:$A$4</formula1>
@@ -1622,7 +1628,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1666,6 +1672,14 @@
       </c>
       <c r="B5" t="s" s="0">
         <v>275</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>276</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -1683,34 +1697,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -1790,10 +1804,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4">
@@ -1806,26 +1820,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8">
@@ -1838,10 +1852,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -1867,18 +1881,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
@@ -1891,10 +1905,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6">
@@ -1915,90 +1929,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2016,42 +2030,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -2069,42 +2083,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2128,16 +2142,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2">
@@ -2145,13 +2159,13 @@
         <v>48</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SBB in the stain name
Closes #52
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="369">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1084,6 +1084,12 @@
     <t>stain_name</t>
   </si>
   <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/LNC/LP6537-7</t>
+  </si>
+  <si>
     <t>Trichrome</t>
   </si>
   <si>
@@ -1342,7 +1348,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-08-03T11:42:07-07:00</t>
+    <t>2024-10-28T09:03:31-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1532,43 +1538,43 @@
         <v>277</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
@@ -1576,7 +1582,7 @@
         <v>50</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1620,7 @@
       <formula1>'is_image_preprocessing_required'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'stain_name'!$A$1:$A$6</formula1>
+      <formula1>'stain_name'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'stain_technique'!$A$1:$A$4</formula1>
@@ -1658,7 +1664,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1710,6 +1716,14 @@
       </c>
       <c r="B6" t="s" s="0">
         <v>289</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1727,10 +1741,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2">
@@ -1743,18 +1757,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1850,26 +1864,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8">
@@ -1882,10 +1896,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1919,10 +1933,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4">
@@ -1935,10 +1949,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6">
@@ -1959,90 +1973,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2068,34 +2082,34 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2113,18 +2127,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3">
@@ -2137,18 +2151,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -2172,16 +2186,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2">
@@ -2189,13 +2203,13 @@
         <v>50</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new acquisition instrument vendor and model
Closes #97
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="433">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -406,6 +406,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -643,6 +649,18 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -763,6 +781,12 @@
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -796,6 +820,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -904,6 +934,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -982,6 +1018,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1132,6 +1174,12 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1492,7 +1540,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:14:37-07:00</t>
+    <t>2025-06-25T11:37:59-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1646,93 +1694,93 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>342</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>342</v>
+        <v>358</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>350</v>
+        <v>366</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>358</v>
+        <v>374</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>385</v>
+        <v>401</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>395</v>
+        <v>411</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>405</v>
+        <v>421</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>406</v>
+        <v>422</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>407</v>
+        <v>423</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>408</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>409</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1741,10 +1789,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$29</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$72</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1816,58 +1864,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>329</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>330</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>331</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>332</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>333</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>335</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>337</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>339</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>340</v>
+        <v>356</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>341</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -1885,34 +1933,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>343</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>344</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>346</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>348</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -1930,12 +1978,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1953,12 +2001,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1976,74 +2024,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>353</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>355</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>357</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -2061,146 +2109,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>361</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>362</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>363</v>
+        <v>379</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>364</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>366</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>368</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>370</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>371</v>
+        <v>387</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>372</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>373</v>
+        <v>389</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>374</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>376</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>377</v>
+        <v>393</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>378</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>379</v>
+        <v>395</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>380</v>
+        <v>396</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>381</v>
+        <v>397</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>382</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>384</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -2218,42 +2266,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>388</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>390</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>392</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>394</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -2271,42 +2319,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>396</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>397</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>399</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>400</v>
+        <v>416</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>401</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>402</v>
+        <v>418</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>403</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -2330,30 +2378,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>410</v>
+        <v>426</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>415</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>416</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2411,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2695,6 +2743,14 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2712,130 +2768,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2853,12 +2909,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2924,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2876,210 +2932,234 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3089,7 +3169,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3097,546 +3177,578 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>301</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>320</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3654,42 +3766,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -3707,26 +3819,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -3744,12 +3856,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a new acquisition instrument model "Panoramic 150 Digital Scanner"
Closes #120
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="458">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -274,34 +274,166 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>CosMx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -310,36 +442,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -370,16 +472,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -388,30 +484,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -442,18 +520,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -466,12 +532,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -484,34 +544,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -775,6 +817,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
@@ -1060,6 +1108,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1150,6 +1204,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1180,6 +1237,12 @@
     <t>https://identifiers.org/RRID:SCR_027095</t>
   </si>
   <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1192,6 +1255,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1216,6 +1285,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1540,7 +1615,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-25T11:37:59-07:00</t>
+    <t>2025-09-25T16:06:39-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1694,93 +1769,93 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>411</v>
+        <v>436</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>424</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>425</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1789,10 +1864,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$29</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$72</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1864,58 +1939,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>349</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>351</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>353</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>355</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>357</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -1933,34 +2008,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>362</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>363</v>
+        <v>388</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>364</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -1978,12 +2053,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2001,12 +2076,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2024,74 +2099,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>369</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>371</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>180</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>373</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -2109,146 +2184,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>376</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>378</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>315</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>380</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>382</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>383</v>
+        <v>408</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>384</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>385</v>
+        <v>410</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>386</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>387</v>
+        <v>412</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>388</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>390</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>391</v>
+        <v>416</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>392</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>394</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>396</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>398</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>400</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2266,42 +2341,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>403</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>404</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>406</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>408</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>409</v>
+        <v>434</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>410</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2319,42 +2394,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>415</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>417</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>419</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -2378,30 +2453,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>429</v>
+        <v>454</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>431</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>430</v>
+        <v>455</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>432</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +2486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2751,6 +2826,62 @@
       </c>
       <c r="B42" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2768,130 +2899,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2909,12 +3040,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2924,7 +3055,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2932,234 +3063,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>150</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>182</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3169,7 +3308,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3177,578 +3316,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>187</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>189</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>191</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>199</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>201</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>207</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>209</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>235</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>255</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>285</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>291</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>301</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>302</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>303</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>155</v>
+        <v>321</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>156</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>307</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>308</v>
+        <v>169</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>309</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>311</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>315</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>317</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>319</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>321</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>325</v>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3766,42 +3945,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>329</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>331</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>333</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>335</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>337</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3819,26 +3998,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>331</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>333</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>335</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3856,12 +4035,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Histology metadata template to use updated field descriptions
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -37,165 +37,178 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>Depending on if the acquisition instrument was a microscope, slide scanner, etc.
-will indicate whether or not any level of preprocessing was required to assemble
-the image (e.g., fusing image tiles) .</t>
+        <t>(Required) Indicates whether image preprocessing is necessary based on the type
+of acquisition instrument used, such as a microscope or slide scanner. This may
+involve steps like fusing image tiles to assemble the complete image. Example:
+Yes</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) The name of the chemical stains (dyes) applied to histology samples
-to highlight important features of the tissue as well as to enhance the tissue
-contrast.</t>
+        <t>(Required) The name of the chemical stains or dyes used on histology samples to
+emphasize key features of the tissue and enhance contrast. Example: H&amp;E</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>There are typically three types of stains: progressive, modified progressive,
-and regressive. Progressive staining occurs when the hematoxylin is added to the
-tissue without being followed by a differentiator to remove excess dye. With
-regressive and modified progressive staining, a differentiator is used.</t>
+        <t>The staining technique used, which can be categorized into three types:
+progressive, modified progressive, and regressive. In progressive staining,
+hematoxylin is applied to the tissue without the use of a differentiator to
+remove excess dye. In contrast, regressive and modified progressive staining
+techniques involve the use of a differentiator. Example: Progressive staining</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) Are the slides stained using a linear batch method or individually?</t>
+        <t>(Required) Indicates whether the slides are stained using a linear batch method
+or individually. Example: No</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>(Required) Is the slide staining automated with an instrument?</t>
+        <t>(Required) Indicates whether the slide staining process is automated using an
+instrument. Example: Yes</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>The manufacturer of the instrument used to prepare (staining/processing) the
-sample for the assay. If an automatic slide staining method was indicated this
-field should list the manufacturer of the instrument.</t>
+        <t>The company that manufactures the instrument used to prepare the sample (e.g.,
+for staining or other processing steps) prior to the assay. If the instrument
+was custom-built or developed internally, enter "In-House". If no sample
+preparation occurred, enter "Not applicable". Example: 10X Genomics</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>Manufacturers of a staining system instrument may offer various versions
-(models) of that instrument with different features. Differences in features or
-sensitivities may be relevant to processing or interpretation of the data.</t>
+        <t>The specific model of the instrument used for sample preparation, such as
+staining. Manufacturers may offer multiple models with varying features or
+sensitivities, which can influence how the sample is processed and how the
+resulting data is interpreted. If no sample preparation occurred, enter "Not
+applicable". Example: Chromium X</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>A unique ID denoting the slide used. This allows users the ability to determine
-which tissue sections were processed together on the same slide. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+        <t>The unique identifier assigned to each slide, enabling users to determine which
+tissue sections were processed together on the same slide. It is recommended
+that data providers prefix the ID with the center name to prevent overlapping
+values across different centers. Example: VAN0071-PA-1-1_AF</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>This is how the tiles are configured for stitching.</t>
+        <t>The configuration of tiles used for stitching in the assay process. If no tile
+configuration is applicable, enter "Not applicable". Example: Row-by-row</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
@@ -205,41 +218,42 @@
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>This is how many columns used in stitching. This is sometimes referred to as the
-grid size x.</t>
+        <t>The number of columns used in the stitching process of a tiled image, often
+referred to as the grid size in the x-dimension. Example: 5</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>This is the total number of raw (tiled) images captured, that are to be stitched
-together.</t>
+        <t>The total number of raw tiled images captured, which are intended to be stitched
+together. Example: 75</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>The amount of overlap between tiled images. This is the set point, where as
-during image acquisition there will be slight variations due to stage
-registration.</t>
+        <t>The intended percentage of overlap between tiled images. This value serves as
+the set point, although slight variations may occur during image acquisition due
+to stage registration. Example: 5</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+        <t>Specifies a semicolon-separated list of non-global files that are to be included
+in the dataset. The file paths assume that the files are located in the
+"TOP/non-global/" directory. For instance, if the file is located at
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson, the value for
+this field would be "./lab_processed/images/1-tissue-boundary.geojson". Once
+ingested, these files will be copied to their appropriate locations within the
+respective dataset directory tree. This field is intended for internal HuBMAP
+processing. Examples for GeoMx and PhenoCycler are provided in the File
+Locations documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee
+Example: ./lab_processed/images/1-tissue-boundary.geojson</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -248,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="460">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -274,6 +288,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
     <t>Visium (no probes)</t>
   </si>
   <si>
@@ -310,24 +330,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>CosMx</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -1615,7 +1635,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-09-25T16:06:39-07:00</t>
+    <t>2025-10-21T14:00:34-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1769,93 +1789,93 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$49</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1939,58 +1959,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2008,34 +2028,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2053,12 +2073,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2076,12 +2096,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2099,74 +2119,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -2184,146 +2204,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2341,42 +2361,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -2394,42 +2414,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -2453,30 +2473,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +2506,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2882,6 +2902,14 @@
       </c>
       <c r="B49" t="s" s="0">
         <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2899,130 +2927,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3040,12 +3068,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3063,242 +3091,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3316,618 +3344,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3945,42 +3973,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3998,26 +4026,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4035,12 +4063,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a new acquisition instrument model NanoZoomer 2.0-RS
Closes #145

Registered the instrument model name as: NanoZoomer 2.0-RS
</commit_message>
<xml_diff>
--- a/histology/latest/histology.xlsx
+++ b/histology/latest/histology.xlsx
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="498">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -367,6 +367,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
+    <t>iCLAP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000479</t>
+  </si>
+  <si>
     <t>seqFISH</t>
   </si>
   <si>
@@ -433,6 +439,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
+    <t>MACSima</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000480</t>
+  </si>
+  <si>
     <t>CyTOF</t>
   </si>
   <si>
@@ -565,6 +577,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
   </si>
   <si>
+    <t>Raman Imaging</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000475</t>
+  </si>
+  <si>
     <t>RNAseq (with probes)</t>
   </si>
   <si>
@@ -577,6 +595,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
+    <t>STARmap</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000476</t>
+  </si>
+  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -604,6 +628,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>Lipid + metabolite + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000478</t>
+  </si>
+  <si>
     <t>RNA + protein</t>
   </si>
   <si>
@@ -790,6 +820,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -844,12 +880,24 @@
     <t>https://identifiers.org/RRID:SCR_023604</t>
   </si>
   <si>
+    <t>Miltenyi Biotec</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008984</t>
+  </si>
+  <si>
     <t>Leica Biosystems</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Revvity</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027779</t>
+  </si>
+  <si>
     <t>Cytek Biosciences</t>
   </si>
   <si>
@@ -979,6 +1027,18 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
+    <t>Opera Phenix Plus HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027780</t>
+  </si>
+  <si>
     <t>timsTOF Pro 2</t>
   </si>
   <si>
@@ -1021,6 +1081,12 @@
     <t>https://identifiers.org/RRID:SCR_027101</t>
   </si>
   <si>
+    <t>Orbitrap Fusion Tribrid</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020559</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1147,6 +1213,18 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
+    <t>Zeiss LightSheet Z.1</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020919</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1219,6 +1297,12 @@
     <t>https://identifiers.org/RRID:SCR_023692</t>
   </si>
   <si>
+    <t>NanoZoomer 2.0-RS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_028001</t>
+  </si>
+  <si>
     <t>Axio Observer 3</t>
   </si>
   <si>
@@ -1288,6 +1372,18 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>SYNAPT G2-Si</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027782</t>
+  </si>
+  <si>
+    <t>MACSima System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027923</t>
+  </si>
+  <si>
     <t>Biomark HD</t>
   </si>
   <si>
@@ -1654,7 +1750,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-20T09:35:57-08:00</t>
+    <t>2026-02-23T12:14:22-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1808,105 +1904,105 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>357</v>
+        <v>389</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>358</v>
+        <v>390</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>369</v>
+        <v>401</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>371</v>
+        <v>403</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>372</v>
+        <v>404</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>374</v>
+        <v>406</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>389</v>
+        <v>421</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>396</v>
+        <v>428</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>397</v>
+        <v>429</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>398</v>
+        <v>430</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>405</v>
+        <v>437</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>434</v>
+        <v>466</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>435</v>
+        <v>467</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>453</v>
+        <v>485</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>454</v>
+        <v>486</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>455</v>
+        <v>487</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>456</v>
+        <v>488</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>457</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>458</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$51</formula1>
+      <formula1>'dataset_type'!$A$1:$A$55</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$17</formula1>
+      <formula1>'analyte_class'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$33</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$85</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1978,58 +2074,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>411</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>413</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>383</v>
+        <v>415</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>384</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>385</v>
+        <v>417</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>386</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>387</v>
+        <v>419</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>388</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -2047,34 +2143,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>390</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>391</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>392</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>393</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>394</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>395</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2092,12 +2188,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2115,12 +2211,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2138,90 +2234,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>399</v>
+        <v>431</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>400</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>401</v>
+        <v>433</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>402</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>202</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>403</v>
+        <v>435</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>404</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -2239,154 +2335,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>406</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>407</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>408</v>
+        <v>440</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>409</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>410</v>
+        <v>442</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>411</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>267</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>343</v>
+        <v>375</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>344</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>412</v>
+        <v>444</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>413</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>414</v>
+        <v>446</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>415</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>416</v>
+        <v>448</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>417</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>418</v>
+        <v>450</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>419</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>421</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>422</v>
+        <v>454</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>423</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>424</v>
+        <v>456</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>425</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>427</v>
+        <v>459</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>429</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>430</v>
+        <v>462</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>431</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>432</v>
+        <v>464</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>433</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -2404,42 +2500,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>436</v>
+        <v>468</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>437</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>438</v>
+        <v>470</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>439</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>440</v>
+        <v>472</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>441</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>443</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -2457,42 +2553,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>446</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>447</v>
+        <v>479</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>448</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>449</v>
+        <v>481</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>450</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>451</v>
+        <v>483</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>452</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -2516,30 +2612,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>464</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>463</v>
+        <v>495</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>465</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -2549,7 +2645,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2963,6 +3059,38 @@
         <v>105</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2970,7 +3098,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2978,138 +3106,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3127,12 +3263,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3142,7 +3278,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3150,242 +3286,266 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>204</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3395,7 +3555,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3403,618 +3563,682 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>207</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>209</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>235</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>255</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>285</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>291</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>301</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>303</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>307</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>309</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>311</v>
+        <v>327</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>313</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>315</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>317</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>319</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>321</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>323</v>
+        <v>339</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>70</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>324</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>326</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>328</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>330</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>175</v>
+        <v>348</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>176</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>332</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>333</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>334</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>336</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>338</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>339</v>
+        <v>357</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>341</v>
+        <v>187</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>342</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>343</v>
+        <v>359</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>344</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>346</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>348</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>352</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>356</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>385</v>
+      </c>
+      <c r="B84" t="s" s="0">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="B85" t="s" s="0">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4032,42 +4256,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>366</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>367</v>
+        <v>399</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>368</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -4085,26 +4309,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>363</v>
+        <v>395</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>364</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>366</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -4122,12 +4346,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>